<commit_message>
Final review of ROB
</commit_message>
<xml_diff>
--- a/review/figures/plot_data/risk_of_bias_data.xlsx
+++ b/review/figures/plot_data/risk_of_bias_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davetaylor/dev/transitions-review/figures/plot_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davetaylor/dev/care-leaver-review/review/figures/plot_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B387DD-ABF7-8F4D-920A-749E8FB8B677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FE7314-858B-5C4B-8359-D24F53A6B332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,15 +206,14 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -245,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -260,9 +259,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -285,21 +281,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,7 +519,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="65.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="12.6640625" style="5" customWidth="1"/>
     <col min="8" max="16384" width="12.6640625" style="5"/>
   </cols>
@@ -560,210 +551,210 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10" t="s">
+      <c r="C4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="10" t="s">
+      <c r="E5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="E6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="E8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="10" t="s">
+      <c r="E9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1772,16 +1763,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA994"/>
+  <dimension ref="A1:J994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="42.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12.6640625" style="5" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
@@ -1791,403 +1782,369 @@
     <col min="10" max="16384" width="12.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="D2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="D3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="18" t="s">
+      <c r="J3" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="18" t="s">
+      <c r="D4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
     </row>
-    <row r="5" spans="1:27" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D6" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="G6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="7" t="s">
+      <c r="H6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="18" t="s">
+      <c r="I6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="17" t="s">
+    <row r="7" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="B7" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="18" t="s">
+      <c r="D7" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="J7" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="17" t="s">
+    <row r="8" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="18" t="s">
+      <c r="B10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="18" t="s">
+      <c r="D10" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H10" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="J10" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J11" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="20"/>
-      <c r="AA7" s="20"/>
     </row>
-    <row r="8" spans="1:27" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="7"/>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>